<commit_message>
updates gastos y canciones
</commit_message>
<xml_diff>
--- a/Gastos_ingresos_calculados_2025.xlsx
+++ b/Gastos_ingresos_calculados_2025.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Allfunds_CB\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CDF6FC-2AAC-47D2-9AF1-524DBB896F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEC37E0-A568-495C-9447-04A0142A2423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gastos_2025" sheetId="2" r:id="rId1"/>
@@ -2039,10 +2039,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I163"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2064,7 +2065,7 @@
         <v>151</v>
       </c>
       <c r="B1" s="8">
-        <v>2169.85</v>
+        <v>1710.68</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -2078,8 +2079,8 @@
         <v>152</v>
       </c>
       <c r="B2" s="8">
-        <f>11545.36-5000</f>
-        <v>6545.3600000000006</v>
+        <f>11493.39-5000</f>
+        <v>6493.3899999999994</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2296,10 +2297,11 @@
       </c>
       <c r="B17" s="18">
         <f>(150*3)-C17</f>
+        <v>150</v>
+      </c>
+      <c r="C17" s="18">
+        <f>150*2</f>
         <v>300</v>
-      </c>
-      <c r="C17" s="18">
-        <v>150</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="2"/>
@@ -2313,11 +2315,11 @@
       </c>
       <c r="B18" s="18">
         <f>(30*4+70*3)-C18</f>
-        <v>190</v>
+        <v>120</v>
       </c>
       <c r="C18" s="18">
-        <f>70*2</f>
-        <v>140</v>
+        <f>70*3</f>
+        <v>210</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="2"/>
@@ -2662,10 +2664,10 @@
       </c>
       <c r="B39" s="28">
         <f>300-C39</f>
+        <v>300</v>
+      </c>
+      <c r="C39" s="28">
         <v>0</v>
-      </c>
-      <c r="C39" s="28">
-        <v>300</v>
       </c>
       <c r="D39" s="48"/>
       <c r="E39" s="2"/>
@@ -2779,11 +2781,11 @@
       </c>
       <c r="B46" s="8">
         <f>SUM(B12:B45)</f>
-        <v>1039.2633333333333</v>
+        <v>1119.2633333333333</v>
       </c>
       <c r="C46" s="8">
         <f>SUM(C12:C30)</f>
-        <v>6511.4800000000005</v>
+        <v>6731.4800000000005</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="2"/>
@@ -2806,7 +2808,7 @@
       </c>
       <c r="B48" s="9">
         <f>SUM(B1:B3)-B46</f>
-        <v>7675.9466666666676</v>
+        <v>7084.8066666666664</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="2"/>
@@ -2827,7 +2829,7 @@
     <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="str">
         <f ca="1">"DEPOSITO EN LITROS A FECHA: "&amp;TEXT(TODAY(),"dd-MM-aaaa")</f>
-        <v>DEPOSITO EN LITROS A FECHA: 07-08-2025</v>
+        <v>DEPOSITO EN LITROS A FECHA: 13-08-2025</v>
       </c>
       <c r="B50" s="17">
         <f>C111</f>
@@ -3857,7 +3859,7 @@
       </c>
       <c r="B115" s="21">
         <f ca="1">TODAY()+B52-5</f>
-        <v>45951.25</v>
+        <v>45957.25</v>
       </c>
       <c r="C115" s="18"/>
       <c r="D115" s="2"/>
@@ -4204,7 +4206,7 @@
       </c>
       <c r="B134" s="5">
         <f ca="1">B115</f>
-        <v>45951.25</v>
+        <v>45957.25</v>
       </c>
       <c r="C134" s="29">
         <v>500</v>
@@ -4552,6 +4554,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Hoja10"/>
   <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5036,6 +5039,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359E7A64-9B40-4277-B45B-9758224AFFD3}">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
@@ -5547,6 +5551,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5822,6 +5827,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6379,6 +6385,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6491,6 +6498,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -6703,6 +6711,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -7113,6 +7122,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Hoja8"/>
   <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView topLeftCell="A71" workbookViewId="0">
@@ -9318,6 +9328,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Hoja9"/>
   <dimension ref="A1:K90"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>